<commit_message>
updated with 14 day, and check inbos
</commit_message>
<xml_diff>
--- a/EmployeeDetails.xlsx
+++ b/EmployeeDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <x:si>
     <x:t>Name of Employee</x:t>
   </x:si>
@@ -108,31 +108,64 @@
     <x:t>Yes</x:t>
   </x:si>
   <x:si>
-    <x:t>sanjay.prajapati@featsystems.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">sanjay </x:t>
-  </x:si>
-  <x:si>
-    <x:t>06/19/2019</x:t>
+    <x:t>mallika.poojari@featsystems.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mallika</x:t>
+  </x:si>
+  <x:si>
+    <x:t>06/21/2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mr.Dhruvin Patel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2nd January 2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21st January 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5,00,000/-pa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Akshay.suryawanshi@featsystems.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Akshay</x:t>
   </x:si>
   <x:si>
     <x:t>Mr.Sanjay Prajapati</x:t>
   </x:si>
   <x:si>
-    <x:t>2nd January 2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21st January 2019</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5,00,000/-pa</x:t>
-  </x:si>
-  <x:si>
-    <x:t>akshay.suryawanshi@featsystems.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Akshay</x:t>
+    <x:t>3rd January 2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22nd January 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8,00,000/-pa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dhruvin.patel@featsystems.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dhruvin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mr.Preety Bhojani</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4th January 2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23rd January 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>preety.bhojani@featsystems.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Preety</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -204,8 +237,8 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -505,17 +538,17 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:R3"/>
+  <x:dimension ref="A1:R5"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <x:selection activeCell="A10" sqref="A10 A10:A10"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="C14" sqref="C14 C14:C14"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.140625" style="6" customWidth="1"/>
+    <x:col min="1" max="1" width="18.710938" style="6" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="20.855469" style="6" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="34.710938" style="6" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="32.710938" style="6" customWidth="1"/>
     <x:col min="4" max="4" width="20.855469" style="6" bestFit="1" customWidth="1"/>
     <x:col min="5" max="5" width="14.285156" style="6" bestFit="1" customWidth="1"/>
     <x:col min="6" max="6" width="24" style="6" bestFit="1" customWidth="1"/>
@@ -527,6 +560,8 @@
     <x:col min="12" max="12" width="46" style="6" bestFit="1" customWidth="1"/>
     <x:col min="13" max="13" width="27.710938" style="6" bestFit="1" customWidth="1"/>
     <x:col min="14" max="14" width="11" style="6" bestFit="1" customWidth="1"/>
+    <x:col min="15" max="16" width="9.140625" style="6" customWidth="1"/>
+    <x:col min="17" max="17" width="11.425781" style="6" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -679,17 +714,114 @@
         <x:v>29</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:18">
-      <x:c r="A10" s="6" t="s"/>
+    <x:row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="6" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B4" s="7" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C4" s="8" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D4" s="6" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E4" s="6" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F4" s="6" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G4" s="6" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="H4" s="6" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I4" s="6" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J4" s="6" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K4" s="6" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="L4" s="6" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="M4" s="9" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N4" s="6" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="O4" s="6" t="s"/>
+      <x:c r="Q4" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="6" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B5" s="7" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C5" s="8" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="D5" s="6" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E5" s="6" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F5" s="6" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G5" s="6" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="H5" s="6" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I5" s="6" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J5" s="6" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K5" s="6" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="L5" s="6" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="M5" s="9" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="N5" s="6" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="Q5" s="6" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:18">
+      <x:c r="C14" s="6" t="s"/>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="M2" r:id="rId7"/>
-    <x:hyperlink ref="M3" r:id="rId8"/>
+    <x:hyperlink ref="M2" r:id="rId10"/>
+    <x:hyperlink ref="M3" r:id="rId11"/>
+    <x:hyperlink ref="M4" r:id="rId12"/>
+    <x:hyperlink ref="M5" r:id="rId13"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>

</xml_diff>